<commit_message>
Implementation in spark 2017-09-06
</commit_message>
<xml_diff>
--- a/data/TB_SENSIB_corr.xlsx
+++ b/data/TB_SENSIB_corr.xlsx
@@ -156,12 +156,6 @@
     <t>ESP_CM_6</t>
   </si>
   <si>
-    <t>ARG_CM_1</t>
-  </si>
-  <si>
-    <t>ARG_CM_2</t>
-  </si>
-  <si>
     <t>ARG_CM_3</t>
   </si>
   <si>
@@ -211,6 +205,12 @@
   </si>
   <si>
     <t>POR_CM_5</t>
+  </si>
+  <si>
+    <t>SCF_ARG_CM_1</t>
+  </si>
+  <si>
+    <t>SCF_ARG_CM_2</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>0.80722519024364003</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>0.83588278166646701</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>0.83588278166646701</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>0.80722519024364003</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>0.83588278166646701</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>0.85426342616498097</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>0.85426342616498097</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B39">
         <v>0.83223983832772097</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B40">
         <v>0.85976983622896097</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B41">
         <v>0.83223983832772097</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B42">
         <v>0.85976983622896097</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43">
         <v>0.87745996405420701</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B55">
         <v>0.79005175822443396</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B56">
         <v>0.79005175822443396</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B57">
         <v>0.79005175822443396</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B58">
         <v>0.79005175822443396</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B59">
         <v>0.79005175822443396</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B60">
         <v>0.79005175822443396</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B61">
         <v>0.79005175822443396</v>

</xml_diff>